<commit_message>
Updated prompt for higher precision
</commit_message>
<xml_diff>
--- a/data/Guide.xlsx
+++ b/data/Guide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matiasibarburu/Desktop/Python/eco395m-Final/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79267\Desktop\eco395m-Final\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE258849-BBB1-604D-83C3-7C40BDEF0278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF34CCA-36F5-4E77-A8E4-BD2FEDCEA8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{84E50151-2F4F-6945-B24F-9857823599D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{84E50151-2F4F-6945-B24F-9857823599D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,35 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Date announced</t>
   </si>
   <si>
-    <t>Seller</t>
-  </si>
-  <si>
     <t>Acquired percentage of the business</t>
   </si>
   <si>
-    <t>Private or public deal?</t>
-  </si>
-  <si>
     <t>Premium (one-day prior the announcement)</t>
   </si>
   <si>
-    <t>Implied Net Debt</t>
-  </si>
-  <si>
-    <t>Form of consideration (cash/stock/debt/mixture)</t>
-  </si>
-  <si>
-    <t>Short deal description</t>
-  </si>
-  <si>
-    <t>Short Business description (target company)</t>
-  </si>
-  <si>
     <t>mm/dd/yyyy</t>
   </si>
   <si>
@@ -83,12 +65,6 @@
     <t xml:space="preserve">Float </t>
   </si>
   <si>
-    <t xml:space="preserve">Accretive or Dilutive </t>
-  </si>
-  <si>
-    <t>Main rationale</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -101,35 +77,63 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Advisor to Seller</t>
-  </si>
-  <si>
-    <t>Advisor to Buyer</t>
-  </si>
-  <si>
-    <t>Industry of Target</t>
-  </si>
-  <si>
-    <t>Implied EV</t>
-  </si>
-  <si>
     <t>Date closed</t>
   </si>
   <si>
-    <t>LTM EBITDA</t>
-  </si>
-  <si>
-    <t>LTM Revenue</t>
-  </si>
-  <si>
     <t>Deal size, mln $</t>
+  </si>
+  <si>
+    <t>Industry of Target (1 or 2 words maximum)</t>
+  </si>
+  <si>
+    <t>Private or public deal? (return 1 word - either public or private)</t>
+  </si>
+  <si>
+    <t>Implied equity value (capitalization of target company - price of one share multiplied by number of target’s shares on the moment of deal announcement)</t>
+  </si>
+  <si>
+    <t>Implied Net Debt (preferrably taken from last balance sheet prior to the deal, calculated as target company's total debt minus cash)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form of consideration (return either all-cash, all-stock, all-debt, mixture (in this case return )  </t>
+  </si>
+  <si>
+    <t>Short deal description (maximum 125 symbols)</t>
+  </si>
+  <si>
+    <t>Revenue for the full year of the announcement date (if no information, take the revenue for the year which preceeded the announcement date)</t>
+  </si>
+  <si>
+    <t>EBITDA (calculated as operating profit plus depreciation) for the full year of the announcement date (if no information, take the revenue for the year which preceeded the announcement date)</t>
+  </si>
+  <si>
+    <t>Short Business description of target company (maximum 125 symbols)</t>
+  </si>
+  <si>
+    <t>Advisor to Target (seller) company (if several advisors were on the deal, return all known)</t>
+  </si>
+  <si>
+    <t>Advisor to Buyer (acquirer) (if several advisors were on the deal, return all known)</t>
+  </si>
+  <si>
+    <t>Accretive or Dilutive deal in the long-term period (return 1 word - either accretive or dilutive)</t>
+  </si>
+  <si>
+    <t>Main rationale (why the acquirer purchased the target? - (maximum 125 symbols))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,14 +159,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{1DC75D89-19E7-409B-9F66-F673F884DE8F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -494,235 +501,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F061C15E-B121-DF45-B377-1CB33FFF48B1}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>